<commit_message>
Alteração dos métodos de módulos, com a inserção do parâmetro driver.
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
+++ b/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriela.nomura\Documents\automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0788B4E0-95ED-453D-9260-1DF000C3FBDA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B427451A-13CF-4E58-B929-B625DBCE12D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">Email </t>
   </si>
@@ -75,9 +75,6 @@
     <t>Gabriela</t>
   </si>
   <si>
-    <t>GabrielaNomura</t>
-  </si>
-  <si>
     <t>Nomura</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>São Paulo</t>
+  </si>
+  <si>
+    <t>"1198145838"</t>
+  </si>
+  <si>
+    <t>"6160450"</t>
+  </si>
+  <si>
+    <t>GabrielaNomura6</t>
   </si>
 </sst>
 </file>
@@ -140,11 +146,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -463,7 +470,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +521,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -529,22 +536,22 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
-        <v>1198145838</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3">
-        <v>6160450</v>
+      <c r="K2" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inserção dos testes de buscas, implementação dos métodos asserts.
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
+++ b/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriela.nomura\Documents\automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B427451A-13CF-4E58-B929-B625DBCE12D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D06E15C-D086-4CC8-BBE2-3A129BBF17EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Teste2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve">Email </t>
   </si>
@@ -93,7 +94,22 @@
     <t>"6160450"</t>
   </si>
   <si>
-    <t>GabrielaNomura6</t>
+    <t>NomeBusca</t>
+  </si>
+  <si>
+    <t>Computador</t>
+  </si>
+  <si>
+    <t>HP ELITEPAD 1000 G2 TABLET</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>BEATS STUDIO 2 OVER-EAR MATTE BLACK HEADPHONES</t>
+  </si>
+  <si>
+    <t>GabrielaNomuraa</t>
   </si>
 </sst>
 </file>
@@ -482,6 +498,8 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -521,7 +539,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -569,4 +587,45 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125F7EDF-7CB7-413C-B4CC-29993401C680}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adição do testng como report e inclusao dos metodos assert
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
+++ b/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriela.nomura\Documents\automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D06E15C-D086-4CC8-BBE2-3A129BBF17EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC54C3B-747C-4107-9B9D-B337D78888E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>NomeBusca</t>
   </si>
   <si>
-    <t>Computador</t>
-  </si>
-  <si>
     <t>HP ELITEPAD 1000 G2 TABLET</t>
   </si>
   <si>
@@ -109,7 +106,10 @@
     <t>BEATS STUDIO 2 OVER-EAR MATTE BLACK HEADPHONES</t>
   </si>
   <si>
-    <t>GabrielaNomuraa</t>
+    <t>HP ELITEBOOK FOLIO</t>
+  </si>
+  <si>
+    <t>GabbrielaNomura</t>
   </si>
 </sst>
 </file>
@@ -608,20 +608,20 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor do teste de cadastro, exclusao do threadsleep, acertos dos reports
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
+++ b/src/br/com/rsinet/hub_TDD/testData/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriela.nomura\Documents\automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC54C3B-747C-4107-9B9D-B337D78888E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6D369F-0A6A-4DA2-A24E-ECD495D85EBC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C4985153-42DC-42E2-B000-666D3A9AB41B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t xml:space="preserve">Email </t>
   </si>
@@ -109,7 +109,34 @@
     <t>HP ELITEBOOK FOLIO</t>
   </si>
   <si>
-    <t>GabbrielaNomura</t>
+    <t>DrGus</t>
+  </si>
+  <si>
+    <t>GabrielaSaraiva</t>
+  </si>
+  <si>
+    <t>GabrielaSantos</t>
+  </si>
+  <si>
+    <t>MAriliaGabriela</t>
+  </si>
+  <si>
+    <t>JoaoPedro</t>
+  </si>
+  <si>
+    <t>Djonga</t>
+  </si>
+  <si>
+    <t>Criolo</t>
+  </si>
+  <si>
+    <t>BacudoExu</t>
+  </si>
+  <si>
+    <t>SheldonNascimento</t>
+  </si>
+  <si>
+    <t>ErikaBadu</t>
   </si>
 </sst>
 </file>
@@ -483,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C515DB9-5A82-4378-AEB3-C2AA09DEC44C}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -572,11 +599,166 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="K3" s="4"/>
+    </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="G6" s="3"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="G10" s="1"/>
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="3"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="G17" s="3"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="G21" s="3"/>
+      <c r="K21" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>